<commit_message>
Corrections sent by Deepthi 3/17/20
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BDEQ/BAU Distribued Electricity Quantities.xlsx
+++ b/InputData/bldgs/BDEQ/BAU Distribued Electricity Quantities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\eps-us-2.1.0\eps-us-2.1.0\InputData\bldgs\BDEQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS India 2.1 - Input Data Revisions_17Mar2020\BDEQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36BE293-F3C4-4123-BC35-70C7819BB62E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B403BE09-F676-43C4-990E-CFCD5AAD8E14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="670" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
   <externalReferences>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="INRLac">[1]Conversions!$E$113</definedName>
@@ -315,7 +314,7 @@
     <t>Distributed Rooftop PV Capacity Factor projections</t>
   </si>
   <si>
-    <t>See variable "DSCF" for more info</t>
+    <t>See variable "bldgs/DSCF" for more info</t>
   </si>
 </sst>
 </file>
@@ -879,130 +878,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="About"/>
-      <sheetName val="India Data"/>
-      <sheetName val="JNNSM Performance data"/>
-      <sheetName val="DSCF"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="15">
-          <cell r="B15">
-            <v>0.17907500000000001</v>
-          </cell>
-          <cell r="C15">
-            <v>0.18271666666666686</v>
-          </cell>
-          <cell r="D15">
-            <v>0.18635833333333363</v>
-          </cell>
-          <cell r="E15">
-            <v>0.19</v>
-          </cell>
-          <cell r="F15">
-            <v>0.1915566666666666</v>
-          </cell>
-          <cell r="G15">
-            <v>0.19311333333333325</v>
-          </cell>
-          <cell r="H15">
-            <v>0.1946699999999999</v>
-          </cell>
-          <cell r="I15">
-            <v>0.19622666666666655</v>
-          </cell>
-          <cell r="J15">
-            <v>0.1977833333333332</v>
-          </cell>
-          <cell r="K15">
-            <v>0.19933999999999985</v>
-          </cell>
-          <cell r="L15">
-            <v>0.2008966666666665</v>
-          </cell>
-          <cell r="M15">
-            <v>0.20245333333333315</v>
-          </cell>
-          <cell r="N15">
-            <v>0.2040099999999998</v>
-          </cell>
-          <cell r="O15">
-            <v>0.20556666666666645</v>
-          </cell>
-          <cell r="P15">
-            <v>0.2071233333333331</v>
-          </cell>
-          <cell r="Q15">
-            <v>0.20867999999999975</v>
-          </cell>
-          <cell r="R15">
-            <v>0.21023666666666641</v>
-          </cell>
-          <cell r="S15">
-            <v>0.21179333333333306</v>
-          </cell>
-          <cell r="T15">
-            <v>0.21335000000000015</v>
-          </cell>
-          <cell r="U15">
-            <v>0.2149066666666668</v>
-          </cell>
-          <cell r="V15">
-            <v>0.21646333333333345</v>
-          </cell>
-          <cell r="W15">
-            <v>0.2180200000000001</v>
-          </cell>
-          <cell r="X15">
-            <v>0.21957666666666675</v>
-          </cell>
-          <cell r="Y15">
-            <v>0.2211333333333334</v>
-          </cell>
-          <cell r="Z15">
-            <v>0.22269000000000005</v>
-          </cell>
-          <cell r="AA15">
-            <v>0.22424666666666671</v>
-          </cell>
-          <cell r="AB15">
-            <v>0.22580333333333336</v>
-          </cell>
-          <cell r="AC15">
-            <v>0.22736000000000001</v>
-          </cell>
-          <cell r="AD15">
-            <v>0.22891666666666666</v>
-          </cell>
-          <cell r="AE15">
-            <v>0.23047333333333331</v>
-          </cell>
-          <cell r="AF15">
-            <v>0.23202999999999996</v>
-          </cell>
-          <cell r="AG15">
-            <v>0.23358666666666661</v>
-          </cell>
-          <cell r="AH15">
-            <v>0.23514333333333326</v>
-          </cell>
-          <cell r="AI15">
-            <v>0.23669999999999991</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1326,9 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5559,8 +5432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1F61ED-AF7C-4F59-9C08-053979BDBD25}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5678,139 +5551,105 @@
         <v>85</v>
       </c>
       <c r="B2" s="45">
-        <f>'[3]India Data'!B15</f>
         <v>0.17907500000000001</v>
       </c>
       <c r="C2" s="45">
-        <f>'[3]India Data'!C15</f>
         <v>0.18271666666666686</v>
       </c>
       <c r="D2" s="45">
-        <f>'[3]India Data'!D15</f>
         <v>0.18635833333333363</v>
       </c>
       <c r="E2" s="45">
-        <f>'[3]India Data'!E15</f>
         <v>0.19</v>
       </c>
       <c r="F2" s="45">
-        <f>'[3]India Data'!F15</f>
         <v>0.1915566666666666</v>
       </c>
       <c r="G2" s="45">
-        <f>'[3]India Data'!G15</f>
         <v>0.19311333333333325</v>
       </c>
       <c r="H2" s="45">
-        <f>'[3]India Data'!H15</f>
         <v>0.1946699999999999</v>
       </c>
       <c r="I2" s="45">
-        <f>'[3]India Data'!I15</f>
         <v>0.19622666666666655</v>
       </c>
       <c r="J2" s="45">
-        <f>'[3]India Data'!J15</f>
         <v>0.1977833333333332</v>
       </c>
       <c r="K2" s="45">
-        <f>'[3]India Data'!K15</f>
         <v>0.19933999999999985</v>
       </c>
       <c r="L2" s="45">
-        <f>'[3]India Data'!L15</f>
         <v>0.2008966666666665</v>
       </c>
       <c r="M2" s="45">
-        <f>'[3]India Data'!M15</f>
         <v>0.20245333333333315</v>
       </c>
       <c r="N2" s="45">
-        <f>'[3]India Data'!N15</f>
         <v>0.2040099999999998</v>
       </c>
       <c r="O2" s="45">
-        <f>'[3]India Data'!O15</f>
         <v>0.20556666666666645</v>
       </c>
       <c r="P2" s="45">
-        <f>'[3]India Data'!P15</f>
         <v>0.2071233333333331</v>
       </c>
       <c r="Q2" s="45">
-        <f>'[3]India Data'!Q15</f>
         <v>0.20867999999999975</v>
       </c>
       <c r="R2" s="45">
-        <f>'[3]India Data'!R15</f>
         <v>0.21023666666666641</v>
       </c>
       <c r="S2" s="45">
-        <f>'[3]India Data'!S15</f>
         <v>0.21179333333333306</v>
       </c>
       <c r="T2" s="45">
-        <f>'[3]India Data'!T15</f>
         <v>0.21335000000000015</v>
       </c>
       <c r="U2" s="45">
-        <f>'[3]India Data'!U15</f>
         <v>0.2149066666666668</v>
       </c>
       <c r="V2" s="45">
-        <f>'[3]India Data'!V15</f>
         <v>0.21646333333333345</v>
       </c>
       <c r="W2" s="45">
-        <f>'[3]India Data'!W15</f>
         <v>0.2180200000000001</v>
       </c>
       <c r="X2" s="45">
-        <f>'[3]India Data'!X15</f>
         <v>0.21957666666666675</v>
       </c>
       <c r="Y2" s="45">
-        <f>'[3]India Data'!Y15</f>
         <v>0.2211333333333334</v>
       </c>
       <c r="Z2" s="45">
-        <f>'[3]India Data'!Z15</f>
         <v>0.22269000000000005</v>
       </c>
       <c r="AA2" s="45">
-        <f>'[3]India Data'!AA15</f>
         <v>0.22424666666666671</v>
       </c>
       <c r="AB2" s="45">
-        <f>'[3]India Data'!AB15</f>
         <v>0.22580333333333336</v>
       </c>
       <c r="AC2" s="45">
-        <f>'[3]India Data'!AC15</f>
         <v>0.22736000000000001</v>
       </c>
       <c r="AD2" s="45">
-        <f>'[3]India Data'!AD15</f>
         <v>0.22891666666666666</v>
       </c>
       <c r="AE2" s="45">
-        <f>'[3]India Data'!AE15</f>
         <v>0.23047333333333331</v>
       </c>
       <c r="AF2" s="45">
-        <f>'[3]India Data'!AF15</f>
         <v>0.23202999999999996</v>
       </c>
       <c r="AG2" s="45">
-        <f>'[3]India Data'!AG15</f>
         <v>0.23358666666666661</v>
       </c>
       <c r="AH2" s="45">
-        <f>'[3]India Data'!AH15</f>
         <v>0.23514333333333326</v>
       </c>
       <c r="AI2" s="45">
-        <f>'[3]India Data'!AI15</f>
         <v>0.23669999999999991</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix error in BDEQ
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BDEQ/BAU Distribued Electricity Quantities.xlsx
+++ b/InputData/bldgs/BDEQ/BAU Distribued Electricity Quantities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chrome Downloads\Internship\eps-india-3.1.3.4\InputData - Low GDP\bldgs\BDEQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\bldgs\BDEQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CCBB2-5CA7-48DE-951B-59047B0F4BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED32F8A4-490A-42E9-B2A8-C8C9F3747AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="670" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1426,27 +1426,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="72.77734375" customWidth="1"/>
-    <col min="5" max="5" width="55.77734375" customWidth="1"/>
+    <col min="2" max="2" width="72.7109375" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="G4" s="49"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1467,14 +1467,14 @@
       </c>
       <c r="G5" s="50"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2015</v>
       </c>
       <c r="E6" s="2"/>
       <c r="G6" s="56"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>43</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="G7" s="50"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>44</v>
       </c>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="G8" s="57"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1501,12 +1501,12 @@
       </c>
       <c r="G9" s="50"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>61</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>49</v>
       </c>
@@ -1522,114 +1522,114 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="58"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E17" s="47"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="42" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>68</v>
       </c>
@@ -1656,13 +1656,13 @@
       <selection activeCell="B2" sqref="B2:AI17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>1736.6455273125823</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3527,17 +3527,17 @@
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>10852.975854387068</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -5437,13 +5437,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
@@ -5459,7 +5459,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -5475,7 +5475,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>2.4519922608094245</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>16.024940863073965</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>42.411501425875059</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -5649,22 +5649,22 @@
         <v>93.317984596770344</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2012</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -5727,34 +5727,34 @@
         <v>13.765424201380537</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -5825,12 +5825,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>51</v>
       </c>
@@ -5847,7 +5847,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -5864,7 +5864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="27" t="s">
         <v>23</v>
@@ -5903,7 +5903,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="32" t="s">
         <v>14</v>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="M34" s="34"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
       <c r="B35" s="36" t="s">
         <v>15</v>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="M35" s="39"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>1.7550915856760183</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>1.6862644646691158</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>10.324068151035402</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>58</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>1943.9738433866296</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>1761.8360586343229</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>11117.429706062809</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>37</v>
       </c>
@@ -6670,7 +6670,7 @@
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -6684,7 +6684,7 @@
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>38</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>40</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B58" s="41">
         <f>DSCF!B2</f>
         <v>0.17907500000000001</v>
@@ -7010,7 +7010,7 @@
         <v>0.23669999999999991</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>4030814.2124714274</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>3653152.9728897978</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -7570,19 +7570,19 @@
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.85899999999999999</v>
       </c>
@@ -7604,13 +7604,13 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B1" s="44">
         <v>2017</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -7831,17 +7831,17 @@
   <dimension ref="A1:AI19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B17" sqref="B17:AI17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="50" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="50"/>
+    <col min="1" max="1" width="25.7109375" style="50" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>97</v>
       </c>
@@ -7858,13 +7858,13 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>89</v>
       </c>
       <c r="G2" s="49"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>38</v>
       </c>
@@ -7905,7 +7905,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
         <v>91</v>
       </c>
@@ -7946,13 +7946,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="53"/>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="53"/>
       <c r="C7" s="53"/>
@@ -7987,7 +7987,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>94</v>
       </c>
@@ -8023,7 +8023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>96</v>
       </c>
@@ -8059,10 +8059,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
         <v>98</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>99</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>102</v>
       </c>
@@ -8169,7 +8169,7 @@
       <c r="AH14" s="5"/>
       <c r="AI14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B15" s="50">
         <v>2017</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>100</v>
       </c>
@@ -8414,109 +8414,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>103</v>
       </c>
       <c r="B17" s="52">
-        <f>B16*1000000</f>
-        <v>-16150921.105627503</v>
+        <f>-B16*1000000</f>
+        <v>16150921.105627503</v>
       </c>
       <c r="C17" s="52">
-        <f t="shared" ref="C17:AI17" si="3">C16*1000000</f>
-        <v>-16871971.580415901</v>
+        <f t="shared" ref="C17:AI17" si="3">-C16*1000000</f>
+        <v>16871971.580415901</v>
       </c>
       <c r="D17" s="52">
         <f t="shared" si="3"/>
-        <v>-17593022.055204302</v>
+        <v>17593022.055204302</v>
       </c>
       <c r="E17" s="52">
         <f t="shared" si="3"/>
-        <v>-18314072.5299927</v>
+        <v>18314072.5299927</v>
       </c>
       <c r="F17" s="52">
         <f t="shared" si="3"/>
-        <v>-19035123.004781097</v>
+        <v>19035123.004781097</v>
       </c>
       <c r="G17" s="52">
         <f t="shared" si="3"/>
-        <v>-19756173.479569498</v>
+        <v>19756173.479569498</v>
       </c>
       <c r="H17" s="52">
         <f t="shared" si="3"/>
-        <v>-19918428.790287238</v>
+        <v>19918428.790287238</v>
       </c>
       <c r="I17" s="52">
         <f t="shared" si="3"/>
-        <v>-20080684.101004977</v>
+        <v>20080684.101004977</v>
       </c>
       <c r="J17" s="52">
         <f t="shared" si="3"/>
-        <v>-20242939.411722772</v>
+        <v>20242939.411722772</v>
       </c>
       <c r="K17" s="52">
         <f t="shared" si="3"/>
-        <v>-20405194.722440571</v>
+        <v>20405194.722440571</v>
       </c>
       <c r="L17" s="52">
         <f t="shared" si="3"/>
-        <v>-20567450.03315831</v>
+        <v>20567450.03315831</v>
       </c>
       <c r="M17" s="52">
         <f t="shared" si="3"/>
-        <v>-20090401.197460778</v>
+        <v>20090401.197460778</v>
       </c>
       <c r="N17" s="52">
         <f t="shared" si="3"/>
-        <v>-19613352.36176319</v>
+        <v>19613352.36176319</v>
       </c>
       <c r="O17" s="52">
         <f t="shared" si="3"/>
-        <v>-19136303.526065603</v>
+        <v>19136303.526065603</v>
       </c>
       <c r="P17" s="52">
         <f t="shared" si="3"/>
-        <v>-18659254.690368015</v>
+        <v>18659254.690368015</v>
       </c>
       <c r="Q17" s="52">
         <f t="shared" si="3"/>
-        <v>-18182205.854670428</v>
+        <v>18182205.854670428</v>
       </c>
       <c r="R17" s="52">
         <f t="shared" si="3"/>
-        <v>-17049526.414044976</v>
+        <v>17049526.414044976</v>
       </c>
       <c r="S17" s="52">
         <f t="shared" si="3"/>
-        <v>-15916846.973419525</v>
+        <v>15916846.973419525</v>
       </c>
       <c r="T17" s="52">
         <f t="shared" si="3"/>
-        <v>-14784167.532794071</v>
+        <v>14784167.532794071</v>
       </c>
       <c r="U17" s="52">
         <f t="shared" si="3"/>
-        <v>-13651488.092168165</v>
+        <v>13651488.092168165</v>
       </c>
       <c r="V17" s="52">
         <f t="shared" si="3"/>
-        <v>-12518808.651542714</v>
+        <v>12518808.651542714</v>
       </c>
       <c r="W17" s="52">
         <f t="shared" si="3"/>
-        <v>-10015046.921233989</v>
+        <v>10015046.921233989</v>
       </c>
       <c r="X17" s="52">
         <f t="shared" si="3"/>
-        <v>-7511285.1909261737</v>
+        <v>7511285.1909261737</v>
       </c>
       <c r="Y17" s="52">
         <f t="shared" si="3"/>
-        <v>-5007523.4606174491</v>
+        <v>5007523.4606174491</v>
       </c>
       <c r="Z17" s="52">
         <f t="shared" si="3"/>
-        <v>-2503761.7303087246</v>
+        <v>2503761.7303087246</v>
       </c>
       <c r="AA17" s="52">
         <f t="shared" si="3"/>
@@ -8555,7 +8555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>101</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>104</v>
       </c>
@@ -8853,13 +8853,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -8966,7 +8966,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -9180,7 +9180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -9394,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -9642,7 +9642,7 @@
         <v>3874615.3487915187</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -9749,7 +9749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -10177,7 +10177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -10498,7 +10498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -10728,13 +10728,13 @@
       <selection activeCell="B15" sqref="B15:AI17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -10948,7 +10948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -11055,7 +11055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -11162,7 +11162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -11376,7 +11376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -11517,7 +11517,7 @@
         <v>3577239.0146497744</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -11624,7 +11624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -11731,7 +11731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -11838,7 +11838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -12052,7 +12052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -12266,7 +12266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -12373,7 +12373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -12480,7 +12480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -12599,18 +12599,17 @@
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:AI11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="35" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="35" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -12717,7 +12716,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -12824,7 +12823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -12931,7 +12930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -13038,7 +13037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -13145,7 +13144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -13252,7 +13251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -13393,7 +13392,7 @@
         <v>22355563.090323985</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -13500,7 +13499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -13607,7 +13606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -13714,109 +13713,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3">
         <f>'Back up generators'!B17</f>
-        <v>-16150921.105627503</v>
+        <v>16150921.105627503</v>
       </c>
       <c r="C11" s="3">
         <f>'Back up generators'!C17</f>
-        <v>-16871971.580415901</v>
+        <v>16871971.580415901</v>
       </c>
       <c r="D11" s="3">
         <f>'Back up generators'!D17</f>
-        <v>-17593022.055204302</v>
+        <v>17593022.055204302</v>
       </c>
       <c r="E11" s="3">
         <f>'Back up generators'!E17</f>
-        <v>-18314072.5299927</v>
+        <v>18314072.5299927</v>
       </c>
       <c r="F11" s="3">
         <f>'Back up generators'!F17</f>
-        <v>-19035123.004781097</v>
+        <v>19035123.004781097</v>
       </c>
       <c r="G11" s="3">
         <f>'Back up generators'!G17</f>
-        <v>-19756173.479569498</v>
+        <v>19756173.479569498</v>
       </c>
       <c r="H11" s="3">
         <f>'Back up generators'!H17</f>
-        <v>-19918428.790287238</v>
+        <v>19918428.790287238</v>
       </c>
       <c r="I11" s="3">
         <f>'Back up generators'!I17</f>
-        <v>-20080684.101004977</v>
+        <v>20080684.101004977</v>
       </c>
       <c r="J11" s="3">
         <f>'Back up generators'!J17</f>
-        <v>-20242939.411722772</v>
+        <v>20242939.411722772</v>
       </c>
       <c r="K11" s="3">
         <f>'Back up generators'!K17</f>
-        <v>-20405194.722440571</v>
+        <v>20405194.722440571</v>
       </c>
       <c r="L11" s="3">
         <f>'Back up generators'!L17</f>
-        <v>-20567450.03315831</v>
+        <v>20567450.03315831</v>
       </c>
       <c r="M11" s="3">
         <f>'Back up generators'!M17</f>
-        <v>-20090401.197460778</v>
+        <v>20090401.197460778</v>
       </c>
       <c r="N11" s="3">
         <f>'Back up generators'!N17</f>
-        <v>-19613352.36176319</v>
+        <v>19613352.36176319</v>
       </c>
       <c r="O11" s="3">
         <f>'Back up generators'!O17</f>
-        <v>-19136303.526065603</v>
+        <v>19136303.526065603</v>
       </c>
       <c r="P11" s="3">
         <f>'Back up generators'!P17</f>
-        <v>-18659254.690368015</v>
+        <v>18659254.690368015</v>
       </c>
       <c r="Q11" s="3">
         <f>'Back up generators'!Q17</f>
-        <v>-18182205.854670428</v>
+        <v>18182205.854670428</v>
       </c>
       <c r="R11" s="3">
         <f>'Back up generators'!R17</f>
-        <v>-17049526.414044976</v>
+        <v>17049526.414044976</v>
       </c>
       <c r="S11" s="3">
         <f>'Back up generators'!S17</f>
-        <v>-15916846.973419525</v>
+        <v>15916846.973419525</v>
       </c>
       <c r="T11" s="3">
         <f>'Back up generators'!T17</f>
-        <v>-14784167.532794071</v>
+        <v>14784167.532794071</v>
       </c>
       <c r="U11" s="3">
         <f>'Back up generators'!U17</f>
-        <v>-13651488.092168165</v>
+        <v>13651488.092168165</v>
       </c>
       <c r="V11" s="3">
         <f>'Back up generators'!V17</f>
-        <v>-12518808.651542714</v>
+        <v>12518808.651542714</v>
       </c>
       <c r="W11" s="3">
         <f>'Back up generators'!W17</f>
-        <v>-10015046.921233989</v>
+        <v>10015046.921233989</v>
       </c>
       <c r="X11" s="3">
         <f>'Back up generators'!X17</f>
-        <v>-7511285.1909261737</v>
+        <v>7511285.1909261737</v>
       </c>
       <c r="Y11" s="3">
         <f>'Back up generators'!Y17</f>
-        <v>-5007523.4606174491</v>
+        <v>5007523.4606174491</v>
       </c>
       <c r="Z11" s="3">
         <f>'Back up generators'!Z17</f>
-        <v>-2503761.7303087246</v>
+        <v>2503761.7303087246</v>
       </c>
       <c r="AA11" s="3">
         <f>'Back up generators'!AA17</f>
@@ -13855,7 +13854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -13962,7 +13961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -14069,7 +14068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -14176,7 +14175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -14283,7 +14282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -14390,7 +14389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -14513,13 +14512,13 @@
       <selection activeCell="B2" sqref="B2:AI17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -14626,7 +14625,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -14733,7 +14732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -14840,7 +14839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -14947,7 +14946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -15054,7 +15053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -15161,7 +15160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -15302,7 +15301,7 @@
         <v>1881.013090816424</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -15409,7 +15408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -15516,7 +15515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -15623,7 +15622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -15730,7 +15729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -15837,7 +15836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -15944,7 +15943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -16051,7 +16050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -16158,7 +16157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -16265,7 +16264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>

</xml_diff>